<commit_message>
just some changes to variables
</commit_message>
<xml_diff>
--- a/renaming.xlsx
+++ b/renaming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamahler/Desktop/SmartRProject/smartproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A57EC-FE5F-334B-B786-8F2EDA6E8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D244A-9990-124F-8D18-904B9B5EAC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="0" windowWidth="12080" windowHeight="21000" xr2:uid="{1AC1F665-0252-A549-9441-9C53A2EAFA46}"/>
   </bookViews>
@@ -5210,8 +5210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EB111D-7913-9646-99BD-391C74ABF1FA}">
   <dimension ref="A1:B784"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>